<commit_message>
"Added data in the Excel sheet"
</commit_message>
<xml_diff>
--- a/data/register_test_data.xlsx
+++ b/data/register_test_data.xlsx
@@ -1,32 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium Python Basics\BDD cucumber\selenium-py-hybridframework\selenium-py-hybridframework\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2D95D8-0D74-4BDC-9302-04F04A3F5E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="11320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="86">
   <si>
     <t>FirstName</t>
   </si>
@@ -43,6 +45,9 @@
     <t>ConfirmPassword</t>
   </si>
   <si>
+    <t>InvalidEmail</t>
+  </si>
+  <si>
     <t>Ravi</t>
   </si>
   <si>
@@ -55,6 +60,9 @@
     <t>Ravi@2024</t>
   </si>
   <si>
+    <t>rktesting.com</t>
+  </si>
+  <si>
     <t>Maria</t>
   </si>
   <si>
@@ -67,6 +75,51 @@
     <t>Maria#321</t>
   </si>
   <si>
+    <t>rktools@mail</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>emily.clark@testmail.com</t>
+  </si>
+  <si>
+    <t>Emi!2025</t>
+  </si>
+  <si>
+    <t>rksystem@.com</t>
+  </si>
+  <si>
+    <t>Omar</t>
+  </si>
+  <si>
+    <t>Farouk</t>
+  </si>
+  <si>
+    <t>omar.farouk@testmail.com</t>
+  </si>
+  <si>
+    <t>Omar#789</t>
+  </si>
+  <si>
+    <t>@gmail.com</t>
+  </si>
+  <si>
+    <t>Kattoju</t>
+  </si>
+  <si>
+    <t>Sunil</t>
+  </si>
+  <si>
+    <t>myfirsttestcase@gmail.com</t>
+  </si>
+  <si>
+    <t>test@123</t>
+  </si>
+  <si>
     <t>Chen</t>
   </si>
   <si>
@@ -91,30 +144,6 @@
     <t>Aa@12345</t>
   </si>
   <si>
-    <t>Emily</t>
-  </si>
-  <si>
-    <t>Clark</t>
-  </si>
-  <si>
-    <t>emily.clark@testmail.com</t>
-  </si>
-  <si>
-    <t>Emi!2025</t>
-  </si>
-  <si>
-    <t>Omar</t>
-  </si>
-  <si>
-    <t>Farouk</t>
-  </si>
-  <si>
-    <t>omar.farouk@testmail.com</t>
-  </si>
-  <si>
-    <t>Omar#789</t>
-  </si>
-  <si>
     <t>Sofia</t>
   </si>
   <si>
@@ -257,33 +286,24 @@
   </si>
   <si>
     <t>Vik@9090</t>
-  </si>
-  <si>
-    <t>InvalidEmail</t>
-  </si>
-  <si>
-    <t>rktesting.com</t>
-  </si>
-  <si>
-    <t>rktools@mail</t>
-  </si>
-  <si>
-    <t>rksystem@.com</t>
-  </si>
-  <si>
-    <t>@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -291,19 +311,348 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -311,28 +660,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -381,7 +1012,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -416,7 +1047,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -590,34 +1221,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.2890625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -634,109 +1260,131 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="F5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>81</v>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{EABD91CB-53D2-42C6-AECB-F77F4B1A4064}"/>
-    <hyperlink ref="F4" r:id="rId2" xr:uid="{F9A86427-5DD1-4A6E-9CE6-3A3D85ACDF09}"/>
+    <hyperlink ref="F3" r:id="rId1" display="rktools@mail"/>
+    <hyperlink ref="F4" r:id="rId2" display="rksystem@.com"/>
+    <hyperlink ref="C6" r:id="rId3" display="myfirsttestcase@gmail.com"/>
+    <hyperlink ref="D6" r:id="rId4" display="test@123"/>
+    <hyperlink ref="E6" r:id="rId4" display="test@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31612F6-AB64-4A77-970A-D3E33D6FDBFC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -753,313 +1401,314 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Register_YW_T2_Verify register functionality with valid data
</commit_message>
<xml_diff>
--- a/data/register_test_data.xlsx
+++ b/data/register_test_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium Python Basics\BDD cucumber\selenium-py-hybridframework\selenium-py-hybridframework\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramesh K\PycharmProjects\ybbank_ui_automationk_1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2D95D8-0D74-4BDC-9302-04F04A3F5E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75342438-9C23-46B9-A8E6-8C5FCA5C7459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
   <si>
     <t>FirstName</t>
   </si>
@@ -259,19 +259,10 @@
     <t>Vik@9090</t>
   </si>
   <si>
-    <t>InvalidEmail</t>
-  </si>
-  <si>
-    <t>rktesting.com</t>
-  </si>
-  <si>
-    <t>rktools@mail</t>
-  </si>
-  <si>
-    <t>rksystem@.com</t>
-  </si>
-  <si>
-    <t>@gmail.com</t>
+    <t>ravi.kumar1@testmail.com</t>
+  </si>
+  <si>
+    <t>maria.lopez2@testmail.com</t>
   </si>
 </sst>
 </file>
@@ -604,7 +595,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,9 +624,6 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -644,17 +632,14 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
+      <c r="C2" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -664,8 +649,8 @@
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
+      <c r="C3" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -673,56 +658,23 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="C4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="C5" s="1"/>
+      <c r="F5" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{EABD91CB-53D2-42C6-AECB-F77F4B1A4064}"/>
-    <hyperlink ref="F4" r:id="rId2" xr:uid="{F9A86427-5DD1-4A6E-9CE6-3A3D85ACDF09}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{65FD0B21-930E-413A-9118-1CE4F45F8B3B}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{E4DAE302-082B-4AD5-892E-10C2ECC11284}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
YW-54-T5_register-match the password and confirm password
</commit_message>
<xml_diff>
--- a/data/register_test_data.xlsx
+++ b/data/register_test_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramesh K\PycharmProjects\ybbank_ui_automationk_1\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srira\PycharmProjects\selenium-py-hybridframework\ybbank_ui_automationk\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75342438-9C23-46B9-A8E6-8C5FCA5C7459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C730646-839D-4902-B264-A8E570BBD87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="80">
   <si>
     <t>FirstName</t>
   </si>
@@ -262,7 +262,10 @@
     <t>ravi.kumar1@testmail.com</t>
   </si>
   <si>
-    <t>maria.lopez2@testmail.com</t>
+    <t>IncorrectPassword</t>
+  </si>
+  <si>
+    <t>Ravi@2025</t>
   </si>
 </sst>
 </file>
@@ -595,20 +598,20 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E4" sqref="A4:E4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -624,8 +627,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -641,37 +647,26 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
+      <c r="F2" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C5" s="1"/>
       <c r="F5" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{65FD0B21-930E-413A-9118-1CE4F45F8B3B}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{E4DAE302-082B-4AD5-892E-10C2ECC11284}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{DEFC0DC7-7A68-4248-9911-92C0124D0136}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -686,9 +681,9 @@
       <selection activeCell="A6" sqref="A6:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -705,7 +700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -722,7 +717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -739,7 +734,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -756,7 +751,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -773,7 +768,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -790,7 +785,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -807,7 +802,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -824,7 +819,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -841,7 +836,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -858,7 +853,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -875,7 +870,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -892,7 +887,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -909,7 +904,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -926,7 +921,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -943,7 +938,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -960,7 +955,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -977,7 +972,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -994,7 +989,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Register with Invalid email
</commit_message>
<xml_diff>
--- a/data/register_test_data.xlsx
+++ b/data/register_test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramesh K\PycharmProjects\ybbank_ui_automationk_1\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ybuiauto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75342438-9C23-46B9-A8E6-8C5FCA5C7459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A524BE79-6047-4665-8838-EC4311E0CDAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="84">
   <si>
     <t>FirstName</t>
   </si>
@@ -263,6 +263,21 @@
   </si>
   <si>
     <t>maria.lopez2@testmail.com</t>
+  </si>
+  <si>
+    <t>Invalid_Email</t>
+  </si>
+  <si>
+    <t>userexample.com</t>
+  </si>
+  <si>
+    <t>user.example.com</t>
+  </si>
+  <si>
+    <t>@domain.com</t>
+  </si>
+  <si>
+    <t>maria.lopez2@stmail.com</t>
   </si>
 </sst>
 </file>
@@ -595,20 +610,20 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E4" sqref="A4:E4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -624,8 +639,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -641,8 +659,11 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -658,13 +679,31 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="F5" s="2"/>
     </row>
@@ -672,9 +711,10 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{65FD0B21-930E-413A-9118-1CE4F45F8B3B}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{E4DAE302-082B-4AD5-892E-10C2ECC11284}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{77AC0137-0BC0-4A4F-A87D-1AB7BBC9481D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -686,9 +726,9 @@
       <selection activeCell="A6" sqref="A6:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -705,7 +745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -722,7 +762,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -739,7 +779,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -756,7 +796,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -773,7 +813,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -790,7 +830,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -807,7 +847,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -824,7 +864,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -841,7 +881,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -858,7 +898,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -875,7 +915,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -892,7 +932,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -909,7 +949,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -926,7 +966,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -943,7 +983,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -960,7 +1000,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -977,7 +1017,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -994,7 +1034,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Updated code changes in Register and test data file
</commit_message>
<xml_diff>
--- a/data/register_test_data.xlsx
+++ b/data/register_test_data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ybuiauto\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramesh K\PycharmProjects\ybbank_ui_automationk_1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A524BE79-6047-4665-8838-EC4311E0CDAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47239020-EB5E-4D73-A540-E1DA14104872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="DuplicateEmail" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
   <si>
     <t>FirstName</t>
   </si>
@@ -609,21 +610,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -643,7 +644,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -663,7 +664,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -683,7 +684,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -703,7 +704,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="F5" s="2"/>
     </row>
@@ -723,12 +724,12 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E7"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -745,7 +746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -762,7 +763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -779,7 +780,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -796,7 +797,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -813,7 +814,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -830,7 +831,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -847,7 +848,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -864,7 +865,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -881,7 +882,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -898,7 +899,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -915,7 +916,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -932,7 +933,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -949,7 +950,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -966,7 +967,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -983,7 +984,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -1000,7 +1001,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -1017,7 +1018,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -1034,7 +1035,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -1054,4 +1055,74 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D977FA-714C-472A-8D81-DF0B60EDB230}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{F015AF26-6290-441B-8006-4179987DE25A}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{1CF20EB6-C55A-40DA-A1C1-25AFF0E9CC8B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test design on YW_T45
</commit_message>
<xml_diff>
--- a/data/register_test_data.xlsx
+++ b/data/register_test_data.xlsx
@@ -1,33 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramesh K\PycharmProjects\ybbank_ui_automationk_1\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47239020-EB5E-4D73-A540-E1DA14104872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="11420" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="DuplicateEmail" sheetId="3" r:id="rId3"/>
+    <sheet name="Fieldsblank" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="84">
   <si>
     <t>FirstName</t>
   </si>
@@ -44,30 +47,51 @@
     <t>ConfirmPassword</t>
   </si>
   <si>
+    <t>Invalid_Email</t>
+  </si>
+  <si>
     <t>Ravi</t>
   </si>
   <si>
     <t>Kumar</t>
   </si>
   <si>
+    <t>ravi.kumar1@testmail.com</t>
+  </si>
+  <si>
+    <t>Ravi@2024</t>
+  </si>
+  <si>
+    <t>userexample.com</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>maria.lopez2@testmail.com</t>
+  </si>
+  <si>
+    <t>Maria#321</t>
+  </si>
+  <si>
+    <t>user.example.com</t>
+  </si>
+  <si>
+    <t>maria.lopez2@stmail.com</t>
+  </si>
+  <si>
+    <t>@domain.com</t>
+  </si>
+  <si>
     <t>ravi.kumar@testmail.com</t>
   </si>
   <si>
-    <t>Ravi@2024</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Lopez</t>
-  </si>
-  <si>
     <t>maria.lopez@testmail.com</t>
   </si>
   <si>
-    <t>Maria#321</t>
-  </si>
-  <si>
     <t>Chen</t>
   </si>
   <si>
@@ -258,39 +282,24 @@
   </si>
   <si>
     <t>Vik@9090</t>
-  </si>
-  <si>
-    <t>ravi.kumar1@testmail.com</t>
-  </si>
-  <si>
-    <t>maria.lopez2@testmail.com</t>
-  </si>
-  <si>
-    <t>Invalid_Email</t>
-  </si>
-  <si>
-    <t>userexample.com</t>
-  </si>
-  <si>
-    <t>user.example.com</t>
-  </si>
-  <si>
-    <t>@domain.com</t>
-  </si>
-  <si>
-    <t>maria.lopez2@stmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -298,19 +307,341 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -318,28 +649,309 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -388,7 +1000,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -423,7 +1035,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -597,34 +1209,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.2890625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -641,95 +1248,96 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3">
       <c r="C5" s="1"/>
-      <c r="F5" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{65FD0B21-930E-413A-9118-1CE4F45F8B3B}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{E4DAE302-082B-4AD5-892E-10C2ECC11284}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{77AC0137-0BC0-4A4F-A87D-1AB7BBC9481D}"/>
+    <hyperlink ref="C2" r:id="rId1" display="ravi.kumar1@testmail.com"/>
+    <hyperlink ref="C3" r:id="rId2" display="maria.lopez2@testmail.com"/>
+    <hyperlink ref="C4" r:id="rId3" display="maria.lopez2@stmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31612F6-AB64-4A77-970A-D3E33D6FDBFC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="A1" sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -746,328 +1354,330 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D977FA-714C-472A-8D81-DF0B60EDB230}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1084,45 +1694,100 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{F015AF26-6290-441B-8006-4179987DE25A}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{1CF20EB6-C55A-40DA-A1C1-25AFF0E9CC8B}"/>
+    <hyperlink ref="C2" r:id="rId1" display="ravi.kumar1@testmail.com"/>
+    <hyperlink ref="C3" r:id="rId1" display="ravi.kumar1@testmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="ravi.kumar1@testmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Register with SQL command in the Email field
</commit_message>
<xml_diff>
--- a/data/register_test_data.xlsx
+++ b/data/register_test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramesh K\PycharmProjects\ybbank_ui_automationk_1\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ybuiauto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47239020-EB5E-4D73-A540-E1DA14104872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68021BBB-5A9B-42D2-988A-8E7D027F6130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
   <si>
     <t>FirstName</t>
   </si>
@@ -263,29 +263,32 @@
     <t>ravi.kumar1@testmail.com</t>
   </si>
   <si>
-    <t>maria.lopez2@testmail.com</t>
-  </si>
-  <si>
     <t>Invalid_Email</t>
   </si>
   <si>
-    <t>userexample.com</t>
-  </si>
-  <si>
-    <t>user.example.com</t>
-  </si>
-  <si>
-    <t>@domain.com</t>
-  </si>
-  <si>
-    <t>maria.lopez2@stmail.com</t>
+    <t>OR 1=1; -- , testuser@example.com</t>
+  </si>
+  <si>
+    <t>admin' DROP TABLE users; -- , random.email123@mail.com</t>
+  </si>
+  <si>
+    <t>saurav.mehta1@testmail.com</t>
+  </si>
+  <si>
+    <t>sofia.fernandez2@testmail.com</t>
+  </si>
+  <si>
+    <t>natalie.khan2@stmail.com</t>
+  </si>
+  <si>
+    <t>{"payload":"' OR 1=1; --","email":"testuser@example.com"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,6 +300,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -323,10 +332,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -610,21 +624,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:E3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -641,10 +655,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -652,7 +666,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -660,11 +674,11 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -672,7 +686,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -680,11 +694,11 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -700,22 +714,17 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="F5" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{65FD0B21-930E-413A-9118-1CE4F45F8B3B}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{E4DAE302-082B-4AD5-892E-10C2ECC11284}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{77AC0137-0BC0-4A4F-A87D-1AB7BBC9481D}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -727,9 +736,9 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -746,7 +755,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -763,7 +772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -780,7 +789,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -797,7 +806,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -814,7 +823,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -831,7 +840,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -848,7 +857,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -865,7 +874,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -882,7 +891,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -899,7 +908,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -916,7 +925,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -933,7 +942,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -950,7 +959,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -967,7 +976,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -984,7 +993,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -1001,7 +1010,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -1018,7 +1027,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -1035,7 +1044,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -1061,13 +1070,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D977FA-714C-472A-8D81-DF0B60EDB230}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1084,7 +1093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1101,7 +1110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
LOG-T28-Verify validation for invalid email format (missing @)
</commit_message>
<xml_diff>
--- a/data/register_test_data.xlsx
+++ b/data/register_test_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramesh K\PycharmProjects\ybbank_ui_automationk_1\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Python\Yuvan_Bank\ybbank_ui_automationk\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47239020-EB5E-4D73-A540-E1DA14104872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C358B257-55E3-4A7F-B722-A6C9291BFCEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
   <si>
     <t>FirstName</t>
   </si>
@@ -279,6 +279,15 @@
   </si>
   <si>
     <t>maria.lopez2@stmail.com</t>
+  </si>
+  <si>
+    <t>Ravi@2025</t>
+  </si>
+  <si>
+    <t>Maria#3215</t>
+  </si>
+  <si>
+    <t>Ravi@20245</t>
   </si>
 </sst>
 </file>
@@ -610,21 +619,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:E3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -644,7 +653,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -654,8 +663,8 @@
       <c r="C2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
+      <c r="D2" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -664,7 +673,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -675,7 +684,7 @@
         <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -684,7 +693,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -694,8 +703,8 @@
       <c r="C4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
+      <c r="D4" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -704,7 +713,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="F5" s="2"/>
     </row>
@@ -713,9 +722,11 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{65FD0B21-930E-413A-9118-1CE4F45F8B3B}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{E4DAE302-082B-4AD5-892E-10C2ECC11284}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{77AC0137-0BC0-4A4F-A87D-1AB7BBC9481D}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{31A0B31E-76B7-4A1D-A124-6297FC82F5A8}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{E9E558DE-9552-4D88-BAC4-4B6E7545C59B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -727,9 +738,9 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -746,7 +757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -763,7 +774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -780,7 +791,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -797,7 +808,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -814,7 +825,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -831,7 +842,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -848,7 +859,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -865,7 +876,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -882,7 +893,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -899,7 +910,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -916,7 +927,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -933,7 +944,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -950,7 +961,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -967,7 +978,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -984,7 +995,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -1001,7 +1012,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -1018,7 +1029,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -1035,7 +1046,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -1061,13 +1072,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D977FA-714C-472A-8D81-DF0B60EDB230}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1084,7 +1100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1094,14 +1110,14 @@
       <c r="C2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
+      <c r="D2" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1111,8 +1127,8 @@
       <c r="C3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
+      <c r="D3" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -1122,6 +1138,8 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F015AF26-6290-441B-8006-4179987DE25A}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{1CF20EB6-C55A-40DA-A1C1-25AFF0E9CC8B}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{BB59B156-49E1-4F9B-9D47-3CBE71165143}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{0E30A883-4254-4114-9B64-DC8A26766BBF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Test design on YW_T67 Test Verify error displayed when password lacks special characters
</commit_message>
<xml_diff>
--- a/data/register_test_data.xlsx
+++ b/data/register_test_data.xlsx
@@ -1,33 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramesh K\PycharmProjects\ybbank_ui_automationk_1\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47239020-EB5E-4D73-A540-E1DA14104872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="11180" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="DuplicateEmail" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="86">
   <si>
     <t>FirstName</t>
   </si>
@@ -44,30 +47,51 @@
     <t>ConfirmPassword</t>
   </si>
   <si>
+    <t>Invalid_Email</t>
+  </si>
+  <si>
     <t>Ravi</t>
   </si>
   <si>
     <t>Kumar</t>
   </si>
   <si>
+    <t>ravi.kumar1@testmail.com</t>
+  </si>
+  <si>
+    <t>Ravi@2024</t>
+  </si>
+  <si>
+    <t>userexample.com</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>maria.lopez2@testmail.com</t>
+  </si>
+  <si>
+    <t>Maria#321</t>
+  </si>
+  <si>
+    <t>user.example.com</t>
+  </si>
+  <si>
+    <t>maria.lopez2@stmail.com</t>
+  </si>
+  <si>
+    <t>@domain.com</t>
+  </si>
+  <si>
     <t>ravi.kumar@testmail.com</t>
   </si>
   <si>
-    <t>Ravi@2024</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Lopez</t>
-  </si>
-  <si>
     <t>maria.lopez@testmail.com</t>
   </si>
   <si>
-    <t>Maria#321</t>
-  </si>
-  <si>
     <t>Chen</t>
   </si>
   <si>
@@ -260,37 +284,28 @@
     <t>Vik@9090</t>
   </si>
   <si>
-    <t>ravi.kumar1@testmail.com</t>
-  </si>
-  <si>
-    <t>maria.lopez2@testmail.com</t>
-  </si>
-  <si>
-    <t>Invalid_Email</t>
-  </si>
-  <si>
-    <t>userexample.com</t>
-  </si>
-  <si>
-    <t>user.example.com</t>
-  </si>
-  <si>
-    <t>@domain.com</t>
-  </si>
-  <si>
-    <t>maria.lopez2@stmail.com</t>
+    <t>Ravi123</t>
+  </si>
+  <si>
+    <t>Ravi2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -298,19 +313,349 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -318,28 +663,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -388,7 +1015,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -423,7 +1050,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -597,34 +1224,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.2890625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -641,95 +1263,98 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2"/>
       <c r="C5" s="1"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{65FD0B21-930E-413A-9118-1CE4F45F8B3B}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{E4DAE302-082B-4AD5-892E-10C2ECC11284}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{77AC0137-0BC0-4A4F-A87D-1AB7BBC9481D}"/>
+    <hyperlink ref="C2" r:id="rId1" display="ravi.kumar1@testmail.com"/>
+    <hyperlink ref="C3" r:id="rId2" display="maria.lopez2@testmail.com"/>
+    <hyperlink ref="C4" r:id="rId3" display="maria.lopez2@stmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31612F6-AB64-4A77-970A-D3E33D6FDBFC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="A1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -746,328 +1371,330 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D977FA-714C-472A-8D81-DF0B60EDB230}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1084,45 +1711,121 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{F015AF26-6290-441B-8006-4179987DE25A}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{1CF20EB6-C55A-40DA-A1C1-25AFF0E9CC8B}"/>
+    <hyperlink ref="C2" r:id="rId1" display="ravi.kumar1@testmail.com"/>
+    <hyperlink ref="C3" r:id="rId1" display="ravi.kumar1@testmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="ravi.kumar1@testmail.com"/>
+    <hyperlink ref="C3" r:id="rId1" display="ravi.kumar1@testmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>